<commit_message>
comparaison modèles machine learning
</commit_message>
<xml_diff>
--- a/stats_modèles.xlsx
+++ b/stats_modèles.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Desktop\UQAC cours\IoT\Projet2_secu_IoT-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{43F044D0-EA2C-412B-A1CA-C21D656276EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18C8EE6-7570-4A4C-9160-78F3D59E5399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats_modèles" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>model</t>
   </si>
@@ -56,12 +56,30 @@
   </si>
   <si>
     <t>MLP</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>DecisionTree</t>
+  </si>
+  <si>
+    <t>RandomForest</t>
+  </si>
+  <si>
+    <t>Machine learning</t>
+  </si>
+  <si>
+    <t>Deep learning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -498,26 +516,65 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
@@ -527,7 +584,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
@@ -535,45 +592,58 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
@@ -581,14 +651,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -639,40 +750,75 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1029,243 +1175,508 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.47265625" customWidth="1"/>
-    <col min="3" max="3" width="10.47265625" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="25">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="25">
         <v>0.95</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="26">
         <v>0.97</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="14"/>
+      <c r="C4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E4" s="25">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="25">
         <v>0.95</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="26">
         <v>0.97</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="14"/>
+      <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11">
+      <c r="E5" s="29">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F5" s="29">
         <v>0.7</v>
       </c>
-      <c r="F5" s="12">
+      <c r="G5" s="30">
         <v>0.83</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="14"/>
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="5">
         <v>0.66</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="6">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="2" t="s">
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="14"/>
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="10">
+      <c r="G7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="14"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="11">
+      <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="E8" s="11">
+      <c r="F8" s="11">
         <v>0.7</v>
       </c>
-      <c r="F8" s="12">
+      <c r="G8" s="12">
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="14"/>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="5">
         <v>0.97</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="14"/>
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="2">
         <v>0.71</v>
       </c>
-      <c r="F10" s="10">
+      <c r="G10" s="8">
         <v>0.83</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="14"/>
+      <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="11">
+      <c r="E11" s="11">
         <v>0.98</v>
       </c>
-      <c r="E11" s="11">
+      <c r="F11" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F11" s="12">
+      <c r="G11" s="12">
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="14"/>
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="5">
         <v>0</v>
       </c>
-      <c r="E12" s="7">
+      <c r="F12" s="5">
         <v>0</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="14"/>
+      <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="9">
+      <c r="F13" s="2">
         <v>0.19</v>
       </c>
-      <c r="F13" s="10">
+      <c r="G13" s="8">
         <v>0.32</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="15"/>
+      <c r="C14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0</v>
       </c>
       <c r="E14" s="11">
         <v>0</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>0</v>
       </c>
-    </row>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="17"/>
+      <c r="C16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="17"/>
+      <c r="C17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="17"/>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="17"/>
+      <c r="C19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="17"/>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="17"/>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="17"/>
+      <c r="C22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="17"/>
+      <c r="C23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.76</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="17"/>
+      <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="17"/>
+      <c r="C25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="18"/>
+      <c r="C26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.76</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
-  <conditionalFormatting sqref="D3:F14">
+  <mergeCells count="2">
+    <mergeCell ref="B15:B26"/>
+    <mergeCell ref="B3:B14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E3:G14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:G26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:G26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1278,5 +1689,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>